<commit_message>
Solve 2023, day 1, part 2
</commit_message>
<xml_diff>
--- a/2023/RuntimesChart.xlsx
+++ b/2023/RuntimesChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\exercises\adventOfCode\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBED25F-EAEB-4299-BB49-F9BAC3814B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E7A75F-71FB-40AC-A036-15A522C4974A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="60" windowWidth="28755" windowHeight="15540" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
   </bookViews>
   <sheets>
     <sheet name="RuntimesChart" sheetId="1" r:id="rId1"/>
@@ -187,10 +187,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>RuntimesChart!$A$3:$A$5</c:f>
+              <c:f>RuntimesChart!$A$3:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -199,24 +199,60 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>RuntimesChart!$B$3:$B$5</c:f>
+              <c:f>RuntimesChart!$B$3:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9.7970799999999997E-3</c:v>
+                  <c:v>8.4891600000000008E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.3944600000000002E-3</c:v>
+                  <c:v>5.7089200000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.951462E-2</c:v>
+                  <c:v>2.4545999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4377800000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1247000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8978459999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1553860000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5758660000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.636104E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1336,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F92283-75AE-4EA8-BD8D-63ABCF1CEF1C}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,7 +1402,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>9.7970799999999997E-3</v>
+        <v>8.4891600000000008E-3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1374,7 +1410,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5.3944600000000002E-3</v>
+        <v>5.7089200000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1382,7 +1418,55 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1.951462E-2</v>
+        <v>2.4545999999999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>3.4377800000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2.1247000000000002E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1.8978459999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1.1553860000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1.5758660000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1.636104E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bug to complete 2023, day 10, part 2
</commit_message>
<xml_diff>
--- a/2023/RuntimesChart.xlsx
+++ b/2023/RuntimesChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\exercises\adventOfCode\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E7A75F-71FB-40AC-A036-15A522C4974A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841530DB-4449-40BD-A8BF-89B9FA17748D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
+    <workbookView xWindow="-23016" yWindow="984" windowWidth="22992" windowHeight="12312" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
   </bookViews>
   <sheets>
     <sheet name="RuntimesChart" sheetId="1" r:id="rId1"/>
@@ -218,6 +218,9 @@
                 <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -228,31 +231,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8.4891600000000008E-3</c:v>
+                  <c:v>4.3167199999999996E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.7089200000000001E-3</c:v>
+                  <c:v>4.0615199999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4545999999999998E-2</c:v>
+                  <c:v>1.3590720000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4377800000000001E-3</c:v>
+                  <c:v>2.11532E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1247000000000002E-3</c:v>
+                  <c:v>4.7965799999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.8978459999999999E-2</c:v>
+                  <c:v>1.539836E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1553860000000001E-2</c:v>
+                  <c:v>1.051E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5758660000000001E-2</c:v>
+                  <c:v>1.1529620000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.636104E-2</c:v>
+                  <c:v>1.5132619999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.10036642</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1372,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F92283-75AE-4EA8-BD8D-63ABCF1CEF1C}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,7 +1408,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>8.4891600000000008E-3</v>
+        <v>4.3167199999999996E-3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1410,7 +1416,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5.7089200000000001E-3</v>
+        <v>4.0615199999999999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1418,7 +1424,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2.4545999999999998E-2</v>
+        <v>1.3590720000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1426,7 +1432,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3.4377800000000001E-3</v>
+        <v>2.11532E-3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1434,7 +1440,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2.1247000000000002E-3</v>
+        <v>4.7965799999999999E-3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1442,7 +1448,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1.8978459999999999E-2</v>
+        <v>1.539836E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1450,7 +1456,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1.1553860000000001E-2</v>
+        <v>1.051E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1458,7 +1464,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1.5758660000000001E-2</v>
+        <v>1.1529620000000001E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1466,7 +1472,15 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1.636104E-2</v>
+        <v>1.5132619999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0.10036642</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solve 2023, day 13 and update outputs
</commit_message>
<xml_diff>
--- a/2023/RuntimesChart.xlsx
+++ b/2023/RuntimesChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\exercises\adventOfCode\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841530DB-4449-40BD-A8BF-89B9FA17748D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B47990-450F-472A-8003-2C4FF5D199CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23016" yWindow="984" windowWidth="22992" windowHeight="12312" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
   </bookViews>
@@ -187,10 +187,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>RuntimesChart!$A$3:$A$13</c:f>
+              <c:f>RuntimesChart!$A$3:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -220,45 +220,63 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>RuntimesChart!$B$3:$B$13</c:f>
+              <c:f>RuntimesChart!$B$3:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>4.3167199999999996E-3</c:v>
+                  <c:v>1.3517380000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0615199999999999E-3</c:v>
+                  <c:v>7.6885399999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3590720000000001E-2</c:v>
+                  <c:v>1.8429040000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.11532E-3</c:v>
+                  <c:v>3.2271800000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.7965799999999999E-3</c:v>
+                  <c:v>4.8616600000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.539836E-2</c:v>
+                  <c:v>2.1164840000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.051E-2</c:v>
+                  <c:v>1.6294039999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1529620000000001E-2</c:v>
+                  <c:v>1.69991E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.5132619999999999E-2</c:v>
+                  <c:v>1.8328480000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.10036642</c:v>
+                  <c:v>0.12447448</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.10642092</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.5150639999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3314400000000002E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1378,10 +1396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F92283-75AE-4EA8-BD8D-63ABCF1CEF1C}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,7 +1426,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4.3167199999999996E-3</v>
+        <v>1.3517380000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1416,7 +1434,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.0615199999999999E-3</v>
+        <v>7.6885399999999998E-3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1424,7 +1442,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1.3590720000000001E-2</v>
+        <v>1.8429040000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1432,7 +1450,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2.11532E-3</v>
+        <v>3.2271800000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1440,7 +1458,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>4.7965799999999999E-3</v>
+        <v>4.8616600000000003E-3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1448,7 +1466,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1.539836E-2</v>
+        <v>2.1164840000000001E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1456,7 +1474,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1.051E-2</v>
+        <v>1.6294039999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1464,7 +1482,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1.1529620000000001E-2</v>
+        <v>1.69991E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1472,7 +1490,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1.5132619999999999E-2</v>
+        <v>1.8328480000000001E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1480,7 +1498,31 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.10036642</v>
+        <v>0.12447448</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0.10642092</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>9.5150639999999995E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>2.3314400000000002E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solve 2023, day 16, part 2
This one could use speeding up.
</commit_message>
<xml_diff>
--- a/2023/RuntimesChart.xlsx
+++ b/2023/RuntimesChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\exercises\adventOfCode\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B47990-450F-472A-8003-2C4FF5D199CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F09205-06A6-43A9-BD5E-53E02F355D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23016" yWindow="984" windowWidth="22992" windowHeight="12312" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
   </bookViews>
@@ -230,6 +230,15 @@
                 <c:pt idx="12">
                   <c:v>13</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -240,43 +249,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1.3517380000000001E-2</c:v>
+                  <c:v>1.610408E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.6885399999999998E-3</c:v>
+                  <c:v>3.1768100000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8429040000000001E-2</c:v>
+                  <c:v>3.043978E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.2271800000000001E-3</c:v>
+                  <c:v>6.5995200000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8616600000000003E-3</c:v>
+                  <c:v>1.0931099999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1164840000000001E-2</c:v>
+                  <c:v>4.096764E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6294039999999999E-2</c:v>
+                  <c:v>2.510078E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.69991E-2</c:v>
+                  <c:v>2.21143E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.8328480000000001E-2</c:v>
+                  <c:v>3.5815520000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.12447448</c:v>
+                  <c:v>0.1863002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.10642092</c:v>
+                  <c:v>0.14555241999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.5150639999999995E-2</c:v>
+                  <c:v>0.136183</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.3314400000000002E-3</c:v>
+                  <c:v>4.2554000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.14823896</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.67006312</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1396,10 +1414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F92283-75AE-4EA8-BD8D-63ABCF1CEF1C}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,7 +1444,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.3517380000000001E-2</v>
+        <v>1.610408E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1434,7 +1452,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>7.6885399999999998E-3</v>
+        <v>3.1768100000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1442,7 +1460,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1.8429040000000001E-2</v>
+        <v>3.043978E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1450,7 +1468,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3.2271800000000001E-3</v>
+        <v>6.5995200000000002E-3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1458,7 +1476,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>4.8616600000000003E-3</v>
+        <v>1.0931099999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1466,7 +1484,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2.1164840000000001E-2</v>
+        <v>4.096764E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1474,7 +1492,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1.6294039999999999E-2</v>
+        <v>2.510078E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1482,7 +1500,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1.69991E-2</v>
+        <v>2.21143E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1490,7 +1508,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1.8328480000000001E-2</v>
+        <v>3.5815520000000003E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1498,7 +1516,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.12447448</v>
+        <v>0.1863002</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1506,7 +1524,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.10642092</v>
+        <v>0.14555241999999999</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1514,7 +1532,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>9.5150639999999995E-2</v>
+        <v>0.136183</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1522,7 +1540,31 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>2.3314400000000002E-3</v>
+        <v>4.2554000000000003E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0.14823896</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>1.67006312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solve 2023, day 18
</commit_message>
<xml_diff>
--- a/2023/RuntimesChart.xlsx
+++ b/2023/RuntimesChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\exercises\adventOfCode\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F09205-06A6-43A9-BD5E-53E02F355D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29A0E90-F1DD-443C-8148-9CED2C5B951D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23016" yWindow="984" windowWidth="22992" windowHeight="12312" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
   </bookViews>
@@ -239,6 +239,12 @@
                 <c:pt idx="15">
                   <c:v>16</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -249,52 +255,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1.610408E-2</c:v>
+                  <c:v>7.29022E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1768100000000001E-2</c:v>
+                  <c:v>4.2787800000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.043978E-2</c:v>
+                  <c:v>1.412152E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5995200000000002E-3</c:v>
+                  <c:v>2.6985400000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0931099999999999E-2</c:v>
+                  <c:v>3.5630000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.096764E-2</c:v>
+                  <c:v>1.3618079999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.510078E-2</c:v>
+                  <c:v>8.7738999999999994E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.21143E-2</c:v>
+                  <c:v>8.0981400000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.5815520000000003E-2</c:v>
+                  <c:v>1.4612119999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1863002</c:v>
+                  <c:v>0.10361328</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.14555241999999999</c:v>
+                  <c:v>5.0498439999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.136183</c:v>
+                  <c:v>7.6046520000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.2554000000000003E-3</c:v>
+                  <c:v>2.2537400000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.14823896</c:v>
+                  <c:v>9.9354559999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>3.5768599999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.67006312</c:v>
+                  <c:v>1.34262456</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.3065276799999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.6119580000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1414,10 +1426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F92283-75AE-4EA8-BD8D-63ABCF1CEF1C}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A3" sqref="A3:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,7 +1456,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.610408E-2</v>
+        <v>7.29022E-3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1452,7 +1464,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3.1768100000000001E-2</v>
+        <v>4.2787800000000003E-3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1460,7 +1472,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3.043978E-2</v>
+        <v>1.412152E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1468,7 +1480,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>6.5995200000000002E-3</v>
+        <v>2.6985400000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1476,7 +1488,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1.0931099999999999E-2</v>
+        <v>3.5630000000000002E-3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1484,7 +1496,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>4.096764E-2</v>
+        <v>1.3618079999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1492,7 +1504,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>2.510078E-2</v>
+        <v>8.7738999999999994E-3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1500,7 +1512,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>2.21143E-2</v>
+        <v>8.0981400000000002E-3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1508,7 +1520,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>3.5815520000000003E-2</v>
+        <v>1.4612119999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1516,7 +1528,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.1863002</v>
+        <v>0.10361328</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1524,7 +1536,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.14555241999999999</v>
+        <v>5.0498439999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1532,7 +1544,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.136183</v>
+        <v>7.6046520000000006E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1540,7 +1552,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>4.2554000000000003E-3</v>
+        <v>2.2537400000000002E-3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1548,7 +1560,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.14823896</v>
+        <v>9.9354559999999995E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1556,7 +1568,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>3.5768599999999998E-3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1564,7 +1576,23 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>1.67006312</v>
+        <v>1.34262456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>3.3065276799999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>1.6119580000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simplify and optimize 2023, day 18
</commit_message>
<xml_diff>
--- a/2023/RuntimesChart.xlsx
+++ b/2023/RuntimesChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\exercises\adventOfCode\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29A0E90-F1DD-443C-8148-9CED2C5B951D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DD09E6-F2D9-4914-BBC8-8F6BE47B531F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23016" yWindow="984" windowWidth="22992" windowHeight="12312" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
   </bookViews>
@@ -255,58 +255,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>7.29022E-3</c:v>
+                  <c:v>1.0450640000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.2787800000000003E-3</c:v>
+                  <c:v>1.6424279999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.412152E-2</c:v>
+                  <c:v>2.2944200000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6985400000000001E-3</c:v>
+                  <c:v>2.9272E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.5630000000000002E-3</c:v>
+                  <c:v>5.7713399999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3618079999999999E-2</c:v>
+                  <c:v>1.1531400000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.7738999999999994E-3</c:v>
+                  <c:v>6.91546E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0981400000000002E-3</c:v>
+                  <c:v>9.4108200000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4612119999999999E-2</c:v>
+                  <c:v>1.3106339999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.10361328</c:v>
+                  <c:v>9.0326660000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.0498439999999999E-2</c:v>
+                  <c:v>4.1978620000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.6046520000000006E-2</c:v>
+                  <c:v>8.4642179999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.2537400000000002E-3</c:v>
+                  <c:v>2.57318E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.9354559999999995E-2</c:v>
+                  <c:v>0.21787583999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.5768599999999998E-3</c:v>
+                  <c:v>8.2094400000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.34262456</c:v>
+                  <c:v>1.70466092</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.3065276799999999</c:v>
+                  <c:v>3.1288574800000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6119580000000001E-2</c:v>
+                  <c:v>1.2481599999999999E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1456,7 +1456,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>7.29022E-3</v>
+        <v>1.0450640000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1464,7 +1464,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.2787800000000003E-3</v>
+        <v>1.6424279999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1472,7 +1472,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1.412152E-2</v>
+        <v>2.2944200000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1480,7 +1480,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2.6985400000000001E-3</v>
+        <v>2.9272E-3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1488,7 +1488,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>3.5630000000000002E-3</v>
+        <v>5.7713399999999998E-3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1496,7 +1496,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1.3618079999999999E-2</v>
+        <v>1.1531400000000001E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1504,7 +1504,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>8.7738999999999994E-3</v>
+        <v>6.91546E-3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1512,7 +1512,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>8.0981400000000002E-3</v>
+        <v>9.4108200000000003E-3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1520,7 +1520,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1.4612119999999999E-2</v>
+        <v>1.3106339999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1528,7 +1528,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.10361328</v>
+        <v>9.0326660000000003E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1536,7 +1536,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>5.0498439999999999E-2</v>
+        <v>4.1978620000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1544,7 +1544,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>7.6046520000000006E-2</v>
+        <v>8.4642179999999997E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1552,7 +1552,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>2.2537400000000002E-3</v>
+        <v>2.57318E-3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1560,7 +1560,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>9.9354559999999995E-2</v>
+        <v>0.21787583999999999</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1568,7 +1568,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>3.5768599999999998E-3</v>
+        <v>8.2094400000000001E-3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>1.34262456</v>
+        <v>1.70466092</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1584,7 +1584,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>3.3065276799999999</v>
+        <v>3.1288574800000002</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1592,7 +1592,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>1.6119580000000001E-2</v>
+        <v>1.2481599999999999E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>